<commit_message>
working on pg 04
</commit_message>
<xml_diff>
--- a/Plymouth_Daily_Rounds.xlsx
+++ b/Plymouth_Daily_Rounds.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="214">
   <si>
     <t>Note: When doing rounds be aware for unusual smells, sounds, sights, or anything not normal.</t>
   </si>
@@ -529,6 +529,15 @@
     <t>Write down the water softener gallon readings from each softener.</t>
   </si>
   <si>
+    <t>Softener#1</t>
+  </si>
+  <si>
+    <t>Softener#2</t>
+  </si>
+  <si>
+    <t>Softener#3</t>
+  </si>
+  <si>
     <t>Well meter reading</t>
   </si>
   <si>
@@ -563,108 +572,6 @@
   </si>
   <si>
     <t>CHW Lakos Bag filter</t>
-  </si>
-  <si>
-    <t>Condenser Supply Temp.  East Side (68 – 85)</t>
-  </si>
-  <si>
-    <t>CWP-6 VFD</t>
-  </si>
-  <si>
-    <t>CWP-1 VFD</t>
-  </si>
-  <si>
-    <t>CWP-4 VFD</t>
-  </si>
-  <si>
-    <t>CWP-3 VFD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDWF  VFD </t>
-  </si>
-  <si>
-    <t>CWP-2 VFD</t>
-  </si>
-  <si>
-    <t>CWP-5 VFD</t>
-  </si>
-  <si>
-    <t>TWR Fan- 6 VFD</t>
-  </si>
-  <si>
-    <t>TWR Fan- 5 VFD</t>
-  </si>
-  <si>
-    <t>CHWR Header Temp East</t>
-  </si>
-  <si>
-    <t>CHWR Temp (Bypass) East</t>
-  </si>
-  <si>
-    <t>Lakos Separator (6psi)</t>
-  </si>
-  <si>
-    <t>CHWS Temp East</t>
-  </si>
-  <si>
-    <t>CHWP #3 VFD</t>
-  </si>
-  <si>
-    <t>Well VFD</t>
-  </si>
-  <si>
-    <t>CHWP #2 VFD</t>
-  </si>
-  <si>
-    <t>CHWP #4 VFD</t>
-  </si>
-  <si>
-    <t>CHWP #1 VFD</t>
-  </si>
-  <si>
-    <t>CHWP #5 VFD</t>
-  </si>
-  <si>
-    <t>EF #6 VFD</t>
-  </si>
-  <si>
-    <t>Core Pump #1 VFD</t>
-  </si>
-  <si>
-    <t>Core Pump #2 VFD</t>
-  </si>
-  <si>
-    <t>HP LL- 3 Ok  (Fan is ok, If there's sweating of pipes check operation of HP)</t>
-  </si>
-  <si>
-    <t>Core Pump #2 (15 - 20 PSID)</t>
-  </si>
-  <si>
-    <t>Core Pump #1 (15 - 20 PSID)</t>
-  </si>
-  <si>
-    <t>Condenser Supply Temp.  West Side (68 – 85)</t>
-  </si>
-  <si>
-    <t>Chemical tanks level (above the order lines)</t>
-  </si>
-  <si>
-    <t>Nalco controller</t>
-  </si>
-  <si>
-    <t>Coupon Rack flow is between 4 – 6 GPM</t>
-  </si>
-  <si>
-    <t>Tower #4 VFD</t>
-  </si>
-  <si>
-    <t>Tower #3 VFD</t>
-  </si>
-  <si>
-    <t>Tower #2 VFD</t>
-  </si>
-  <si>
-    <t>Tower #1 VFD</t>
   </si>
   <si>
     <t>Tear off sticky mat (Battery Room)</t>
@@ -945,7 +852,7 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="6" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1008,9 +915,21 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2031,28 +1950,28 @@
     </row>
     <row customHeight="1" ht="16" r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="16" t="n"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E2" s="16" t="n"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="33" t="s">
         <v>76</v>
       </c>
       <c r="G2" s="16" t="n"/>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="33" t="s">
         <v>76</v>
       </c>
       <c r="I2" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="16" r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>10</v>
@@ -2081,7 +2000,7 @@
     </row>
     <row customHeight="1" ht="16" r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>10</v>
@@ -2110,28 +2029,28 @@
     </row>
     <row customHeight="1" ht="16" r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="C5" s="16" t="n"/>
       <c r="D5" s="19" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="E5" s="16" t="n"/>
       <c r="F5" s="19" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="G5" s="16" t="n"/>
       <c r="H5" s="19" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="I5" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="16" r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>10</v>
@@ -2160,7 +2079,7 @@
     </row>
     <row customHeight="1" ht="16" r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>10</v>
@@ -2181,7 +2100,7 @@
     </row>
     <row customHeight="1" ht="16" r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>10</v>
@@ -2202,7 +2121,7 @@
     </row>
     <row customHeight="1" ht="16" r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>10</v>
@@ -2223,7 +2142,7 @@
     </row>
     <row customHeight="1" ht="16" r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>10</v>
@@ -2244,7 +2163,7 @@
     </row>
     <row customHeight="1" ht="16" r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>10</v>
@@ -2273,7 +2192,7 @@
     </row>
     <row customHeight="1" ht="16" r="12" spans="1:9">
       <c r="A12" s="16" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>10</v>
@@ -2302,7 +2221,7 @@
     </row>
     <row customHeight="1" ht="16" r="13" spans="1:9">
       <c r="A13" s="16" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>10</v>
@@ -2331,7 +2250,7 @@
     </row>
     <row customHeight="1" ht="16" r="14" spans="1:9">
       <c r="A14" s="16" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>10</v>
@@ -2352,7 +2271,7 @@
     </row>
     <row customHeight="1" ht="16" r="15" spans="1:9">
       <c r="A15" s="16" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>10</v>
@@ -2373,7 +2292,7 @@
     </row>
     <row customHeight="1" ht="16" r="16" spans="1:9">
       <c r="A16" s="16" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>10</v>
@@ -2402,7 +2321,7 @@
     </row>
     <row customHeight="1" ht="16" r="17" spans="1:9">
       <c r="A17" s="16" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>10</v>
@@ -2460,9 +2379,9 @@
     </row>
     <row customHeight="1" ht="16" r="19" spans="1:9">
       <c r="A19" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="B19" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="16" t="n"/>
@@ -2470,32 +2389,32 @@
         <v>10</v>
       </c>
       <c r="E19" s="16" t="n"/>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="34" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="16" t="n"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>10</v>
       </c>
       <c r="I19" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="16" r="20" spans="1:9">
       <c r="A20" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B20" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="33" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="16" t="n"/>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="16" t="n"/>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="33" t="s">
         <v>76</v>
       </c>
       <c r="G20" s="16" t="n"/>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="33" t="s">
         <v>76</v>
       </c>
       <c r="I20" s="16" t="n"/>
@@ -2515,28 +2434,28 @@
     </row>
     <row customHeight="1" ht="16" r="22" spans="1:9">
       <c r="A22" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="B22" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="33" t="s">
         <v>76</v>
       </c>
       <c r="C22" s="16" t="n"/>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E22" s="16" t="n"/>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="33" t="s">
         <v>76</v>
       </c>
       <c r="G22" s="16" t="n"/>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="33" t="s">
         <v>76</v>
       </c>
       <c r="I22" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="16" r="23" spans="1:9">
       <c r="A23" s="16" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>10</v>
@@ -2565,7 +2484,7 @@
     </row>
     <row customHeight="1" ht="16" r="24" spans="1:9">
       <c r="A24" s="16" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>10</v>
@@ -2594,7 +2513,7 @@
     </row>
     <row customHeight="1" ht="16" r="25" spans="1:9">
       <c r="A25" s="16" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>10</v>
@@ -2623,7 +2542,7 @@
     </row>
     <row customHeight="1" ht="16" r="26" spans="1:9">
       <c r="A26" s="16" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>10</v>
@@ -2644,7 +2563,7 @@
     </row>
     <row customHeight="1" ht="16" r="27" spans="1:9">
       <c r="A27" s="16" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>10</v>
@@ -2665,7 +2584,7 @@
     </row>
     <row customHeight="1" ht="16" r="28" spans="1:9">
       <c r="A28" s="16" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>10</v>
@@ -2686,7 +2605,7 @@
     </row>
     <row customHeight="1" ht="16" r="29" spans="1:9">
       <c r="A29" s="16" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>10</v>
@@ -2707,7 +2626,7 @@
     </row>
     <row customHeight="1" ht="16" r="30" spans="1:9">
       <c r="A30" s="16" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>10</v>
@@ -2736,7 +2655,7 @@
     </row>
     <row customHeight="1" ht="16" r="31" spans="1:9">
       <c r="A31" s="16" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>10</v>
@@ -2765,7 +2684,7 @@
     </row>
     <row customHeight="1" ht="16" r="32" spans="1:9">
       <c r="A32" s="16" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>10</v>
@@ -2794,7 +2713,7 @@
     </row>
     <row customHeight="1" ht="16" r="33" spans="1:9">
       <c r="A33" s="16" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>10</v>
@@ -2823,7 +2742,7 @@
     </row>
     <row customHeight="1" ht="16" r="34" spans="1:9">
       <c r="A34" s="16" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>10</v>
@@ -2883,7 +2802,7 @@
       <c r="A36" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="16" t="n"/>
@@ -2891,39 +2810,39 @@
         <v>10</v>
       </c>
       <c r="E36" s="16" t="n"/>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="34" t="s">
         <v>10</v>
       </c>
       <c r="G36" s="16" t="n"/>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="34" t="s">
         <v>10</v>
       </c>
       <c r="I36" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="16" r="37" spans="1:9">
       <c r="A37" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="B37" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="16" t="n"/>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E37" s="16" t="n"/>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="33" t="s">
         <v>76</v>
       </c>
       <c r="G37" s="16" t="n"/>
-      <c r="H37" s="27" t="s">
+      <c r="H37" s="33" t="s">
         <v>76</v>
       </c>
       <c r="I37" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="38" spans="1:9">
       <c r="A38" s="14" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="B38" s="12" t="n"/>
       <c r="C38" s="16" t="n"/>
@@ -4969,7 +4888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4984,798 +4903,491 @@
     <col customWidth="1" max="5" min="5" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:5">
+      <c r="A1" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="16" t="n"/>
-      <c r="C1" s="16" t="n"/>
-      <c r="D1" s="16" t="n"/>
-      <c r="E1" s="16" t="n"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="16" t="s">
+      <c r="B1" s="31" t="n"/>
+      <c r="C1" s="31" t="n"/>
+      <c r="D1" s="31" t="n"/>
+      <c r="E1" s="31" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="2" spans="1:5">
+      <c r="A2" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="16" t="n"/>
-      <c r="C2" s="16" t="n"/>
-      <c r="D2" s="16" t="n"/>
-      <c r="E2" s="16" t="n"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="32" t="n"/>
+      <c r="D2" s="32" t="n"/>
+      <c r="E2" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="3" spans="1:5">
+      <c r="A3" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="16" t="n"/>
-      <c r="C3" s="16" t="n"/>
-      <c r="D3" s="16" t="n"/>
-      <c r="E3" s="16" t="n"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="16" t="s">
+      <c r="B3" s="32" t="n"/>
+      <c r="C3" s="32" t="n"/>
+      <c r="D3" s="32" t="n"/>
+      <c r="E3" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="4" spans="1:5">
+      <c r="A4" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="16" t="n"/>
-      <c r="C4" s="16" t="n"/>
-      <c r="D4" s="16" t="n"/>
-      <c r="E4" s="16" t="n"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="26" t="s">
+      <c r="B4" s="32" t="n"/>
+      <c r="C4" s="32" t="n"/>
+      <c r="D4" s="32" t="n"/>
+      <c r="E4" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="5" spans="1:5">
+      <c r="A5" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="16" t="n"/>
-      <c r="C5" s="16" t="n"/>
-      <c r="D5" s="16" t="n"/>
-      <c r="E5" s="16" t="n"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="32" t="n"/>
+      <c r="C5" s="32" t="n"/>
+      <c r="D5" s="32" t="n"/>
+      <c r="E5" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="6" spans="1:5">
+      <c r="A6" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="16" t="n"/>
-      <c r="C6" s="16" t="n"/>
-      <c r="D6" s="16" t="n"/>
-      <c r="E6" s="16" t="n"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="16" t="s">
+      <c r="B6" s="32" t="n"/>
+      <c r="C6" s="32" t="n"/>
+      <c r="D6" s="32" t="n"/>
+      <c r="E6" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="7" spans="1:5">
+      <c r="A7" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="16" t="n"/>
-      <c r="C7" s="16" t="n"/>
-      <c r="D7" s="16" t="n"/>
-      <c r="E7" s="16" t="n"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="16" t="s">
+      <c r="B7" s="32" t="n"/>
+      <c r="C7" s="32" t="n"/>
+      <c r="D7" s="32" t="n"/>
+      <c r="E7" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="8" spans="1:5">
+      <c r="A8" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="16" t="n"/>
-      <c r="C8" s="16" t="n"/>
-      <c r="D8" s="16" t="n"/>
-      <c r="E8" s="16" t="n"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="16" t="s">
+      <c r="B8" s="32" t="n"/>
+      <c r="C8" s="32" t="n"/>
+      <c r="D8" s="32" t="n"/>
+      <c r="E8" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="9" spans="1:5">
+      <c r="A9" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="16" t="n"/>
-      <c r="C9" s="16" t="n"/>
-      <c r="D9" s="16" t="n"/>
-      <c r="E9" s="16" t="n"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="16" t="s">
+      <c r="B9" s="32" t="n"/>
+      <c r="C9" s="32" t="n"/>
+      <c r="D9" s="32" t="n"/>
+      <c r="E9" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="10" spans="1:5">
+      <c r="A10" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="16" t="n"/>
-      <c r="C10" s="16" t="n"/>
-      <c r="D10" s="16" t="n"/>
-      <c r="E10" s="16" t="n"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="16" t="s">
+      <c r="B10" s="32" t="n"/>
+      <c r="C10" s="32" t="n"/>
+      <c r="D10" s="32" t="n"/>
+      <c r="E10" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="11" spans="1:5">
+      <c r="A11" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="16" t="n"/>
-      <c r="C11" s="16" t="n"/>
-      <c r="D11" s="16" t="n"/>
-      <c r="E11" s="16" t="n"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="17" t="s">
+      <c r="B11" s="32" t="n"/>
+      <c r="C11" s="32" t="n"/>
+      <c r="D11" s="32" t="n"/>
+      <c r="E11" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="12" spans="1:5">
+      <c r="A12" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="16" t="n"/>
-      <c r="C12" s="16" t="n"/>
-      <c r="D12" s="16" t="n"/>
-      <c r="E12" s="16" t="n"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="26" t="s">
+      <c r="B12" s="31" t="n"/>
+      <c r="C12" s="31" t="n"/>
+      <c r="D12" s="31" t="n"/>
+      <c r="E12" s="31" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="13" spans="1:5">
+      <c r="A13" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="16" t="n"/>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="32" t="n"/>
+      <c r="D13" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="E13" s="16" t="n"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="16" t="n"/>
-      <c r="B14" s="16" t="s">
+      <c r="E13" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="14" spans="1:5">
+      <c r="A14" s="32" t="n"/>
+      <c r="B14" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="16" t="n"/>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="32" t="n"/>
+      <c r="D14" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="E14" s="16" t="n"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="16" t="n"/>
-      <c r="B15" s="16" t="s">
+      <c r="E14" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="15" spans="1:5">
+      <c r="A15" s="32" t="n"/>
+      <c r="B15" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="16" t="n"/>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="32" t="n"/>
+      <c r="D15" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="16" t="n"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="16" t="n"/>
-      <c r="B16" s="16" t="s">
+      <c r="E15" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="16" spans="1:5">
+      <c r="A16" s="32" t="n"/>
+      <c r="B16" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="16" t="n"/>
-      <c r="B17" s="16" t="s">
+      <c r="C16" s="32" t="n"/>
+      <c r="D16" s="32" t="n"/>
+      <c r="E16" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="17" spans="1:5">
+      <c r="A17" s="32" t="n"/>
+      <c r="B17" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="16" t="n"/>
-      <c r="D17" s="16" t="n"/>
-      <c r="E17" s="16" t="n"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="16" t="n"/>
-      <c r="B18" s="16" t="s">
+      <c r="C17" s="32" t="n"/>
+      <c r="D17" s="32" t="n"/>
+      <c r="E17" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="24" r="18" spans="1:5">
+      <c r="A18" s="32" t="n"/>
+      <c r="B18" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="16" t="n"/>
-      <c r="D18" s="16" t="n"/>
-      <c r="E18" s="16" t="n"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="16" t="s">
+      <c r="C18" s="32" t="n"/>
+      <c r="D18" s="32" t="n"/>
+      <c r="E18" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="19" spans="1:5">
+      <c r="A19" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="16" t="n"/>
-      <c r="C19" s="16" t="n"/>
-      <c r="D19" s="16" t="n"/>
-      <c r="E19" s="16" t="n"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="16" t="s">
+      <c r="B19" s="32" t="n"/>
+      <c r="C19" s="32" t="n"/>
+      <c r="D19" s="32" t="n"/>
+      <c r="E19" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" spans="1:5">
+      <c r="A20" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="16" t="n"/>
-      <c r="C20" s="16" t="n"/>
-      <c r="D20" s="16" t="n"/>
-      <c r="E20" s="16" t="n"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="16" t="s">
+      <c r="B20" s="32" t="n"/>
+      <c r="C20" s="32" t="n"/>
+      <c r="D20" s="32" t="n"/>
+      <c r="E20" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" spans="1:5">
+      <c r="A21" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="16" t="n"/>
-      <c r="C21" s="16" t="n"/>
-      <c r="D21" s="16" t="n"/>
-      <c r="E21" s="16" t="n"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="16" t="s">
+      <c r="B21" s="32" t="n"/>
+      <c r="C21" s="32" t="n"/>
+      <c r="D21" s="32" t="n"/>
+      <c r="E21" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" spans="1:5">
+      <c r="A22" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="16" t="n"/>
-      <c r="C22" s="16" t="n"/>
-      <c r="D22" s="16" t="n"/>
-      <c r="E22" s="16" t="n"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="16" t="s">
+      <c r="B22" s="32" t="n"/>
+      <c r="C22" s="32" t="n"/>
+      <c r="D22" s="32" t="n"/>
+      <c r="E22" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" spans="1:5">
+      <c r="A23" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B23" s="16" t="n"/>
-      <c r="C23" s="16" t="n"/>
-      <c r="D23" s="16" t="n"/>
-      <c r="E23" s="16" t="n"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="16" t="s">
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="32" t="n"/>
+      <c r="D23" s="32" t="n"/>
+      <c r="E23" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" spans="1:5">
+      <c r="A24" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="16" t="n"/>
-      <c r="C24" s="16" t="n"/>
-      <c r="D24" s="16" t="n"/>
-      <c r="E24" s="16" t="n"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="16" t="s">
+      <c r="B24" s="32" t="n"/>
+      <c r="C24" s="32" t="n"/>
+      <c r="D24" s="32" t="n"/>
+      <c r="E24" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="25" spans="1:5">
+      <c r="A25" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="16" t="n"/>
-      <c r="C25" s="16" t="n"/>
-      <c r="D25" s="16" t="n"/>
-      <c r="E25" s="16" t="n"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="16" t="s">
+      <c r="B25" s="32" t="n"/>
+      <c r="C25" s="32" t="n"/>
+      <c r="D25" s="32" t="n"/>
+      <c r="E25" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="26" spans="1:5">
+      <c r="A26" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="16" t="n"/>
-      <c r="C26" s="16" t="n"/>
-      <c r="D26" s="16" t="n"/>
-      <c r="E26" s="16" t="n"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="16" t="s">
+      <c r="B26" s="32" t="n"/>
+      <c r="C26" s="32" t="n"/>
+      <c r="D26" s="32" t="n"/>
+      <c r="E26" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="27" spans="1:5">
+      <c r="A27" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B27" s="16" t="n"/>
-      <c r="C27" s="16" t="n"/>
-      <c r="D27" s="16" t="n"/>
-      <c r="E27" s="16" t="n"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="17" t="s">
+      <c r="B27" s="32" t="n"/>
+      <c r="C27" s="32" t="n"/>
+      <c r="D27" s="32" t="n"/>
+      <c r="E27" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="28" spans="1:5">
+      <c r="A28" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="16" t="n"/>
-      <c r="C28" s="16" t="n"/>
-      <c r="D28" s="16" t="n"/>
-      <c r="E28" s="16" t="n"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="16" t="s">
+      <c r="B28" s="31" t="n"/>
+      <c r="C28" s="31" t="n"/>
+      <c r="D28" s="31" t="n"/>
+      <c r="E28" s="31" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="29" spans="1:5">
+      <c r="A29" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="16" t="n"/>
-      <c r="C29" s="16" t="n"/>
-      <c r="D29" s="16" t="n"/>
-      <c r="E29" s="16" t="n"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="26" t="s">
+      <c r="B29" s="32" t="n"/>
+      <c r="C29" s="32" t="n"/>
+      <c r="D29" s="32" t="n"/>
+      <c r="E29" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="30" spans="1:5">
+      <c r="A30" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="16" t="n"/>
-      <c r="C30" s="16" t="n"/>
-      <c r="D30" s="16" t="n"/>
-      <c r="E30" s="16" t="n"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="16" t="s">
+      <c r="B30" s="32" t="n"/>
+      <c r="C30" s="32" t="n"/>
+      <c r="D30" s="32" t="n"/>
+      <c r="E30" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="31" spans="1:5">
+      <c r="A31" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="16" t="n"/>
-      <c r="C31" s="16" t="n"/>
-      <c r="D31" s="16" t="n"/>
-      <c r="E31" s="16" t="n"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="16" t="s">
+      <c r="B31" s="32" t="n"/>
+      <c r="C31" s="32" t="n"/>
+      <c r="D31" s="32" t="n"/>
+      <c r="E31" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="32" spans="1:5">
+      <c r="A32" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="16" t="n"/>
-      <c r="C32" s="16" t="n"/>
-      <c r="D32" s="16" t="n"/>
-      <c r="E32" s="16" t="n"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="16" t="s">
+      <c r="B32" s="31" t="n"/>
+      <c r="C32" s="31" t="n"/>
+      <c r="D32" s="31" t="n"/>
+      <c r="E32" s="31" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="33" spans="1:5">
+      <c r="A33" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B33" s="16" t="n"/>
-      <c r="C33" s="16" t="n"/>
-      <c r="D33" s="16" t="n"/>
-      <c r="E33" s="16" t="n"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="26" t="s">
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="32" t="n"/>
+      <c r="D33" s="32" t="n"/>
+      <c r="E33" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="34" spans="1:5">
+      <c r="A34" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="16" t="n"/>
-      <c r="C34" s="16" t="n"/>
-      <c r="D34" s="16" t="n"/>
-      <c r="E34" s="16" t="n"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="16" t="n"/>
-      <c r="B35" s="16" t="n"/>
-      <c r="C35" s="16" t="n"/>
-      <c r="D35" s="16" t="n"/>
-      <c r="E35" s="16" t="n"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="16" t="n"/>
-      <c r="B36" s="16" t="n"/>
-      <c r="C36" s="16" t="n"/>
-      <c r="D36" s="16" t="n"/>
-      <c r="E36" s="16" t="n"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="16" t="s">
+      <c r="B34" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="16" t="n"/>
-      <c r="C37" s="16" t="n"/>
-      <c r="D37" s="16" t="n"/>
-      <c r="E37" s="16" t="n"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="16" t="s">
+      <c r="C34" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="35" spans="1:5">
+      <c r="A35" s="32" t="n"/>
+      <c r="B35" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="16" t="n"/>
-      <c r="C38" s="16" t="n"/>
-      <c r="D38" s="16" t="n"/>
-      <c r="E38" s="16" t="n"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="16" t="s">
+      <c r="C35" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="36" spans="1:5">
+      <c r="A36" s="32" t="n"/>
+      <c r="B36" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="16" t="n"/>
-      <c r="C39" s="16" t="n"/>
-      <c r="D39" s="16" t="n"/>
-      <c r="E39" s="16" t="n"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="16" t="s">
+      <c r="C36" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="37" spans="1:5">
+      <c r="A37" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="16" t="n"/>
-      <c r="C40" s="16" t="n"/>
-      <c r="D40" s="16" t="n"/>
-      <c r="E40" s="16" t="n"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="16" t="s">
+      <c r="B37" s="32" t="n"/>
+      <c r="C37" s="32" t="n"/>
+      <c r="D37" s="32" t="n"/>
+      <c r="E37" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="38" spans="1:5">
+      <c r="A38" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="16" t="n"/>
-      <c r="C41" s="16" t="n"/>
-      <c r="D41" s="16" t="n"/>
-      <c r="E41" s="16" t="n"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="16" t="s">
+      <c r="B38" s="32" t="n"/>
+      <c r="C38" s="32" t="n"/>
+      <c r="D38" s="32" t="n"/>
+      <c r="E38" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="39" spans="1:5">
+      <c r="A39" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="16" t="n"/>
-      <c r="C42" s="16" t="n"/>
-      <c r="D42" s="16" t="n"/>
-      <c r="E42" s="16" t="n"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="16" t="s">
+      <c r="B39" s="32" t="n"/>
+      <c r="C39" s="32" t="n"/>
+      <c r="D39" s="32" t="n"/>
+      <c r="E39" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="40" spans="1:5">
+      <c r="A40" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B43" s="16" t="n"/>
-      <c r="C43" s="16" t="n"/>
-      <c r="D43" s="16" t="n"/>
-      <c r="E43" s="16" t="n"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="16" t="s">
+      <c r="B40" s="32" t="n"/>
+      <c r="C40" s="32" t="n"/>
+      <c r="D40" s="32" t="n"/>
+      <c r="E40" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="41" spans="1:5">
+      <c r="A41" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="B44" s="16" t="n"/>
-      <c r="C44" s="16" t="n"/>
-      <c r="D44" s="16" t="n"/>
-      <c r="E44" s="16" t="n"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="16" t="s">
+      <c r="B41" s="32" t="n"/>
+      <c r="C41" s="32" t="n"/>
+      <c r="D41" s="32" t="n"/>
+      <c r="E41" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="42" spans="1:5">
+      <c r="A42" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="16" t="n"/>
-      <c r="C45" s="16" t="n"/>
-      <c r="D45" s="16" t="n"/>
-      <c r="E45" s="16" t="n"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="16" t="s">
+      <c r="B42" s="32" t="n"/>
+      <c r="C42" s="32" t="n"/>
+      <c r="D42" s="32" t="n"/>
+      <c r="E42" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="43" spans="1:5">
+      <c r="A43" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B46" s="16" t="n"/>
-      <c r="C46" s="16" t="n"/>
-      <c r="D46" s="16" t="n"/>
-      <c r="E46" s="16" t="n"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="16" t="s">
+      <c r="B43" s="32" t="n"/>
+      <c r="C43" s="32" t="n"/>
+      <c r="D43" s="32" t="n"/>
+      <c r="E43" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="44" spans="1:5">
+      <c r="A44" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="B47" s="16" t="n"/>
-      <c r="C47" s="16" t="n"/>
-      <c r="D47" s="16" t="n"/>
-      <c r="E47" s="16" t="n"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="16" t="s">
+      <c r="B44" s="32" t="n"/>
+      <c r="C44" s="32" t="n"/>
+      <c r="D44" s="32" t="n"/>
+      <c r="E44" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="45" spans="1:5">
+      <c r="A45" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="16" t="n"/>
-      <c r="C48" s="16" t="n"/>
-      <c r="D48" s="16" t="n"/>
-      <c r="E48" s="16" t="n"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="16" t="s">
+      <c r="B45" s="32" t="n"/>
+      <c r="C45" s="32" t="n"/>
+      <c r="D45" s="32" t="n"/>
+      <c r="E45" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="46" spans="1:5">
+      <c r="A46" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="B49" s="16" t="n"/>
-      <c r="C49" s="16" t="n"/>
-      <c r="D49" s="16" t="n"/>
-      <c r="E49" s="16" t="n"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="16" t="s">
+      <c r="B46" s="32" t="n"/>
+      <c r="C46" s="32" t="n"/>
+      <c r="D46" s="32" t="n"/>
+      <c r="E46" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="47" spans="1:5">
+      <c r="A47" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="16" t="n"/>
-      <c r="C50" s="16" t="n"/>
-      <c r="D50" s="16" t="n"/>
-      <c r="E50" s="16" t="n"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="16" t="s">
+      <c r="B47" s="32" t="n"/>
+      <c r="C47" s="32" t="n"/>
+      <c r="D47" s="32" t="n"/>
+      <c r="E47" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="48" spans="1:5">
+      <c r="A48" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="B51" s="16" t="n"/>
-      <c r="C51" s="16" t="n"/>
-      <c r="D51" s="16" t="n"/>
-      <c r="E51" s="16" t="n"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B52" s="16" t="n"/>
-      <c r="C52" s="16" t="n"/>
-      <c r="D52" s="16" t="n"/>
-      <c r="E52" s="16" t="n"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B53" s="16" t="n"/>
-      <c r="C53" s="16" t="n"/>
-      <c r="D53" s="16" t="n"/>
-      <c r="E53" s="16" t="n"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="B54" s="16" t="n"/>
-      <c r="C54" s="16" t="n"/>
-      <c r="D54" s="16" t="n"/>
-      <c r="E54" s="16" t="n"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="B55" s="16" t="n"/>
-      <c r="C55" s="16" t="n"/>
-      <c r="D55" s="16" t="n"/>
-      <c r="E55" s="16" t="n"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="B56" s="16" t="n"/>
-      <c r="C56" s="16" t="n"/>
-      <c r="D56" s="16" t="n"/>
-      <c r="E56" s="16" t="n"/>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="B57" s="16" t="n"/>
-      <c r="C57" s="16" t="n"/>
-      <c r="D57" s="16" t="n"/>
-      <c r="E57" s="16" t="n"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="B58" s="16" t="n"/>
-      <c r="C58" s="16" t="n"/>
-      <c r="D58" s="16" t="n"/>
-      <c r="E58" s="16" t="n"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B59" s="16" t="n"/>
-      <c r="C59" s="16" t="n"/>
-      <c r="D59" s="16" t="n"/>
-      <c r="E59" s="16" t="n"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B60" s="16" t="n"/>
-      <c r="C60" s="16" t="n"/>
-      <c r="D60" s="16" t="n"/>
-      <c r="E60" s="16" t="n"/>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B61" s="16" t="n"/>
-      <c r="C61" s="16" t="n"/>
-      <c r="D61" s="16" t="n"/>
-      <c r="E61" s="16" t="n"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="B62" s="16" t="n"/>
-      <c r="C62" s="16" t="n"/>
-      <c r="D62" s="16" t="n"/>
-      <c r="E62" s="16" t="n"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="B63" s="16" t="n"/>
-      <c r="C63" s="16" t="n"/>
-      <c r="D63" s="16" t="n"/>
-      <c r="E63" s="16" t="n"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="B64" s="16" t="n"/>
-      <c r="C64" s="16" t="n"/>
-      <c r="D64" s="16" t="n"/>
-      <c r="E64" s="16" t="n"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="B65" s="16" t="n"/>
-      <c r="C65" s="16" t="n"/>
-      <c r="D65" s="16" t="n"/>
-      <c r="E65" s="16" t="n"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B66" s="16" t="n"/>
-      <c r="C66" s="16" t="n"/>
-      <c r="D66" s="16" t="n"/>
-      <c r="E66" s="16" t="n"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B67" s="16" t="n"/>
-      <c r="C67" s="16" t="n"/>
-      <c r="D67" s="16" t="n"/>
-      <c r="E67" s="16" t="n"/>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="B68" s="16" t="n"/>
-      <c r="C68" s="16" t="n"/>
-      <c r="D68" s="16" t="n"/>
-      <c r="E68" s="16" t="n"/>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="B69" s="16" t="n"/>
-      <c r="C69" s="16" t="n"/>
-      <c r="D69" s="16" t="n"/>
-      <c r="E69" s="16" t="n"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="B70" s="16" t="n"/>
-      <c r="C70" s="16" t="n"/>
-      <c r="D70" s="16" t="n"/>
-      <c r="E70" s="16" t="n"/>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="B71" s="16" t="n"/>
-      <c r="C71" s="16" t="n"/>
-      <c r="D71" s="16" t="n"/>
-      <c r="E71" s="16" t="n"/>
+      <c r="B48" s="32" t="n"/>
+      <c r="C48" s="32" t="n"/>
+      <c r="D48" s="32" t="n"/>
+      <c r="E48" s="32" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="49" spans="1:5">
+      <c r="A49" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="32" t="n"/>
+      <c r="C49" s="32" t="n"/>
+      <c r="D49" s="32" t="n"/>
+      <c r="E49" s="32" t="n"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="B72" s="16" t="n"/>
-      <c r="C72" s="16" t="n"/>
-      <c r="D72" s="16" t="n"/>
-      <c r="E72" s="16" t="n"/>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="B73" s="16" t="n"/>
-      <c r="C73" s="16" t="n"/>
-      <c r="D73" s="16" t="n"/>
-      <c r="E73" s="16" t="n"/>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="B74" s="16" t="n"/>
-      <c r="C74" s="16" t="n"/>
-      <c r="D74" s="16" t="n"/>
-      <c r="E74" s="16" t="n"/>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="B75" s="16" t="n"/>
-      <c r="C75" s="16" t="n"/>
-      <c r="D75" s="16" t="n"/>
-      <c r="E75" s="16" t="n"/>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="B76" s="16" t="n"/>
-      <c r="C76" s="16" t="n"/>
-      <c r="D76" s="16" t="n"/>
-      <c r="E76" s="16" t="n"/>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B77" s="16" t="n"/>
-      <c r="C77" s="16" t="n"/>
-      <c r="D77" s="16" t="n"/>
-      <c r="E77" s="16" t="n"/>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B78" s="16" t="n"/>
-      <c r="C78" s="16" t="n"/>
-      <c r="D78" s="16" t="n"/>
-      <c r="E78" s="16" t="n"/>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="B79" s="16" t="n"/>
-      <c r="C79" s="16" t="n"/>
-      <c r="D79" s="16" t="n"/>
-      <c r="E79" s="16" t="n"/>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" t="s">
-        <v>46</v>
-      </c>
+      <c r="A72" s="29" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="12">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A27:E27"/>
     <mergeCell ref="A28:E28"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A32:E32"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
     <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A34:A36"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>